<commit_message>
Se comitea una version estable del desarrollo.
</commit_message>
<xml_diff>
--- a/excel/envio.xlsx
+++ b/excel/envio.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5EC004-1A06-456B-9A0A-B7B849CC0FE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED81A8B-038F-7140-AA3D-C4379F7951CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>76107191-2</t>
   </si>
   <si>
     <t>rut</t>
+  </si>
+  <si>
+    <t>77011330-K</t>
+  </si>
+  <si>
+    <t>76201998-1</t>
+  </si>
+  <si>
+    <t>76220748-6</t>
   </si>
 </sst>
 </file>
@@ -343,57 +352,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>